<commit_message>
Add dark/light mode toggle
</commit_message>
<xml_diff>
--- a/Translations.xlsx
+++ b/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Scripts\Javascript\AnilistCustomListManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD9D451-A9CB-44B8-A152-6FFB997C3AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC6438F-7D62-47DC-A260-A597C05B55DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="1103">
   <si>
     <t>msgid</t>
   </si>
@@ -814,9 +814,6 @@
     <t>set to true and not associated with any custom lists will not be returned by the query and will not be displayed here.</t>
   </si>
   <si>
-    <t>establecidas en true y no asociadas a ninguna lista personalizada no serán devueltas por la consulta y no se mostrarán aquí.</t>
-  </si>
-  <si>
     <t>text.total_entries_updated</t>
   </si>
   <si>
@@ -1381,12 +1378,6 @@
     <t>Chargement...</t>
   </si>
   <si>
-    <t>Note : Les entrées des médias avec</t>
-  </si>
-  <si>
-    <t>ayant la valeur « true » et n'étant pas associés à des listes personnalisées ne seront pas renvoyés par la requête et ne seront pas affichés ici.</t>
-  </si>
-  <si>
     <t>Total des entrées mises à jour :</t>
   </si>
   <si>
@@ -1780,15 +1771,6 @@
     <t>該当なし</t>
   </si>
   <si>
-    <t>注意: メディアエントリーで</t>
-  </si>
-  <si>
-    <t>hiddenFromStatusListsが</t>
-  </si>
-  <si>
-    <t>が true に設定され、カスタムリストに関連付けられていないメディアエントリは、クエリによって返されず、ここには表示されません。</t>
-  </si>
-  <si>
     <t>総エントリ更新数</t>
   </si>
   <si>
@@ -2140,12 +2122,6 @@
     <t>不适用</t>
   </si>
   <si>
-    <t>注：媒体条目带有</t>
-  </si>
-  <si>
-    <t>设置为 “true ”且未与任何自定义列表关联的媒体条目不会被查询返回，也不会在此显示。</t>
-  </si>
-  <si>
     <t>已更新条目总数：</t>
   </si>
   <si>
@@ -3211,9 +3187,6 @@
     <t>참고: 미디어 항목에</t>
   </si>
   <si>
-    <t>숨겨진상태목록</t>
-  </si>
-  <si>
     <t>가 true로 설정되어 있고 사용자 지정 목록과 연결되지 않은 미디어 항목은 쿼리에서 반환되지 않으며 여기에 표시되지 않습니다.</t>
   </si>
   <si>
@@ -3332,6 +3305,30 @@
   </si>
   <si>
     <t>업데이트 중</t>
+  </si>
+  <si>
+    <t>en true y no asociadas a ninguna lista personalizada no serán devueltas por la consulta y no se mostrarán aquí.</t>
+  </si>
+  <si>
+    <t>Note : Les entrées de médias avec</t>
+  </si>
+  <si>
+    <t>sont définies sur true et ne sont pas associées à des listes personnalisées ne seront pas renvoyées par la requête et ne seront pas affichées ici.</t>
+  </si>
+  <si>
+    <t>注：以下のメディアエントリー</t>
+  </si>
+  <si>
+    <t>がtrueに設定され、カスタムリストに関連付けられていないメディアエントリは、クエリによって返されず、ここには表示されません。</t>
+  </si>
+  <si>
+    <t>注：带有</t>
+  </si>
+  <si>
+    <t>设置为 “true ”且未与任何自定义列表关联的媒体条目将不会被查询返回，也不会在此显示。</t>
+  </si>
+  <si>
+    <t>숨겨진 상태 목록</t>
   </si>
 </sst>
 </file>
@@ -3776,8 +3773,8 @@
   </sheetPr>
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I132" sqref="I2:I132"/>
+    <sheetView tabSelected="1" topLeftCell="F72" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3804,22 +3801,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>981</v>
+        <v>973</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3833,22 +3830,22 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>982</v>
+        <v>974</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3862,22 +3859,22 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>983</v>
+        <v>975</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3891,22 +3888,22 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>984</v>
+        <v>976</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3920,22 +3917,22 @@
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>985</v>
+        <v>977</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3949,22 +3946,22 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>986</v>
+        <v>978</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3978,22 +3975,22 @@
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>987</v>
+        <v>979</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4007,22 +4004,22 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>988</v>
+        <v>980</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4036,22 +4033,22 @@
         <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>989</v>
+        <v>981</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4065,22 +4062,22 @@
         <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4094,22 +4091,22 @@
         <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>991</v>
+        <v>983</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4123,22 +4120,22 @@
         <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4152,22 +4149,22 @@
         <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4181,22 +4178,22 @@
         <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4213,7 +4210,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>43</v>
@@ -4225,7 +4222,7 @@
         <v>43</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>995</v>
+        <v>987</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4242,7 +4239,7 @@
         <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>45</v>
@@ -4254,7 +4251,7 @@
         <v>45</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>996</v>
+        <v>988</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4271,10 +4268,10 @@
         <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>47</v>
@@ -4300,10 +4297,10 @@
         <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>50</v>
@@ -4326,22 +4323,22 @@
         <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>997</v>
+        <v>989</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4355,22 +4352,22 @@
         <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4384,22 +4381,22 @@
         <v>57</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>998</v>
+        <v>990</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4416,13 +4413,13 @@
         <v>59</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>59</v>
@@ -4442,22 +4439,22 @@
         <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>999</v>
+        <v>991</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4471,22 +4468,22 @@
         <v>65</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>1000</v>
+        <v>992</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4500,19 +4497,19 @@
         <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>67</v>
@@ -4529,22 +4526,22 @@
         <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1001</v>
+        <v>993</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4558,22 +4555,22 @@
         <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>1002</v>
+        <v>994</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4587,22 +4584,22 @@
         <v>77</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>1003</v>
+        <v>995</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4616,22 +4613,22 @@
         <v>80</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>1004</v>
+        <v>996</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4645,22 +4642,22 @@
         <v>83</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1005</v>
+        <v>997</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4674,22 +4671,22 @@
         <v>86</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4706,19 +4703,19 @@
         <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4732,22 +4729,22 @@
         <v>92</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>1008</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4761,22 +4758,22 @@
         <v>95</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>1009</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4790,22 +4787,22 @@
         <v>98</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>1010</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4822,7 +4819,7 @@
         <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>100</v>
@@ -4834,7 +4831,7 @@
         <v>100</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>1011</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4848,22 +4845,22 @@
         <v>103</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>103</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>1012</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4877,22 +4874,22 @@
         <v>106</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>1013</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4906,22 +4903,22 @@
         <v>109</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>1002</v>
+        <v>994</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4935,22 +4932,22 @@
         <v>83</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>1005</v>
+        <v>997</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4964,22 +4961,22 @@
         <v>114</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>1014</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -4993,22 +4990,22 @@
         <v>117</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>1015</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5022,22 +5019,22 @@
         <v>120</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>1016</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5051,22 +5048,22 @@
         <v>123</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>1017</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5080,22 +5077,22 @@
         <v>126</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>1018</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -5109,22 +5106,22 @@
         <v>129</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>1019</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5138,22 +5135,22 @@
         <v>132</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>1020</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5167,22 +5164,22 @@
         <v>135</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>1021</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5196,22 +5193,22 @@
         <v>138</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>1022</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5225,22 +5222,22 @@
         <v>141</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>1023</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5254,22 +5251,22 @@
         <v>144</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>1024</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5283,22 +5280,22 @@
         <v>146</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>1025</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5312,22 +5309,22 @@
         <v>149</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>1026</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5341,22 +5338,22 @@
         <v>152</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>1027</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5370,22 +5367,22 @@
         <v>155</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>1028</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -5399,22 +5396,22 @@
         <v>158</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>1029</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5428,22 +5425,22 @@
         <v>161</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>1030</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5457,22 +5454,22 @@
         <v>164</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>1031</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5486,22 +5483,22 @@
         <v>167</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>1032</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5515,22 +5512,22 @@
         <v>170</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>1033</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5544,22 +5541,22 @@
         <v>173</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>1034</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5573,22 +5570,22 @@
         <v>176</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1035</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5602,22 +5599,22 @@
         <v>179</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>1036</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5631,22 +5628,22 @@
         <v>182</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1037</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5660,22 +5657,22 @@
         <v>185</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>184</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>1038</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -5689,22 +5686,22 @@
         <v>188</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>1039</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5718,22 +5715,22 @@
         <v>191</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>1040</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5747,22 +5744,22 @@
         <v>194</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>1041</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5776,22 +5773,22 @@
         <v>197</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>1042</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5805,22 +5802,22 @@
         <v>200</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>1043</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5834,22 +5831,22 @@
         <v>203</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>1044</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="72" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5863,22 +5860,22 @@
         <v>206</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>1045</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5892,22 +5889,22 @@
         <v>209</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>1046</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5921,22 +5918,22 @@
         <v>212</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>1047</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5950,22 +5947,22 @@
         <v>215</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>1048</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5979,22 +5976,22 @@
         <v>218</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>1049</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6008,22 +6005,22 @@
         <v>221</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>1050</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6037,22 +6034,22 @@
         <v>224</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>1051</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6066,22 +6063,22 @@
         <v>227</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1052</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6095,22 +6092,22 @@
         <v>230</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>1053</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6124,22 +6121,22 @@
         <v>233</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>1054</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -6153,22 +6150,22 @@
         <v>236</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>1055</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6182,22 +6179,22 @@
         <v>239</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6211,22 +6208,22 @@
         <v>242</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>1057</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6240,22 +6237,22 @@
         <v>245</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>1058</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6269,22 +6266,22 @@
         <v>248</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>1059</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6298,22 +6295,22 @@
         <v>251</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1060</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6327,22 +6324,22 @@
         <v>254</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>1061</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6359,10 +6356,10 @@
         <v>256</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="G89" s="1" t="s">
         <v>256</v>
@@ -6385,22 +6382,22 @@
         <v>259</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>453</v>
+        <v>1096</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>586</v>
+        <v>1098</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>706</v>
+        <v>1100</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1062</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -6417,7 +6414,7 @@
         <v>261</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>587</v>
+        <v>261</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>261</v>
@@ -6429,7 +6426,7 @@
         <v>261</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>1063</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -6440,668 +6437,668 @@
         <v>263</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>264</v>
+        <v>1095</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>454</v>
+        <v>1097</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>588</v>
+        <v>1099</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>707</v>
+        <v>1101</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>1064</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>267</v>
-      </c>
       <c r="D93" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>1065</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="D94" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>1066</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="D95" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>1067</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="D96" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>1068</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="D97" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>1069</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="D98" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>1070</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>285</v>
-      </c>
       <c r="D99" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>1071</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="D100" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>1072</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="D101" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>1073</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>294</v>
-      </c>
       <c r="D102" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>1074</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>1075</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="D104" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>1076</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>301</v>
-      </c>
       <c r="D105" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>1077</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>1078</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>307</v>
-      </c>
       <c r="D107" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>1079</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>310</v>
-      </c>
       <c r="D108" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>1080</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>313</v>
-      </c>
       <c r="D109" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>1081</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B110" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="C110" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>316</v>
-      </c>
       <c r="D110" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>1082</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="D111" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>1083</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="C112" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="D112" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>1084</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>1085</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="D114" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>1086</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>146</v>
@@ -7110,518 +7107,519 @@
         <v>146</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>1025</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>373</v>
-      </c>
       <c r="D116" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>964</v>
+        <v>956</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>1087</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="C117" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>965</v>
+        <v>957</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>1088</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="118" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>334</v>
-      </c>
       <c r="D118" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>966</v>
+        <v>958</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>1089</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B119" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="D119" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>967</v>
+        <v>959</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>1090</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B120" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C120" s="3" t="s">
-        <v>340</v>
-      </c>
       <c r="D120" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>1091</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="121" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>343</v>
-      </c>
       <c r="D121" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>969</v>
+        <v>961</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>1092</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B122" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="C122" s="3" t="s">
-        <v>346</v>
-      </c>
       <c r="D122" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>970</v>
+        <v>962</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>1093</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="123" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B123" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="C123" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>349</v>
-      </c>
       <c r="D123" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>971</v>
+        <v>963</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>1094</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="124" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B124" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="C124" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>352</v>
-      </c>
       <c r="D124" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>972</v>
+        <v>964</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>1095</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>973</v>
+        <v>965</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>1096</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="126" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="C126" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="C126" s="3" t="s">
-        <v>357</v>
-      </c>
       <c r="D126" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>974</v>
+        <v>966</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>1097</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="127" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>975</v>
+        <v>967</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>1098</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>976</v>
+        <v>968</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>1099</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="129" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B129" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="C129" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>362</v>
-      </c>
       <c r="D129" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>977</v>
+        <v>969</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>1100</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="130" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="C130" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="C130" s="3" t="s">
-        <v>365</v>
-      </c>
       <c r="D130" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>978</v>
+        <v>970</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>1101</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="131" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="C131" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="C131" s="3" t="s">
-        <v>368</v>
-      </c>
       <c r="D131" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>979</v>
+        <v>971</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>1102</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="132" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="C132" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C132" s="3" t="s">
-        <v>371</v>
-      </c>
       <c r="D132" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>980</v>
+        <v>972</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>1103</v>
+        <v>1094</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>